<commit_message>
added Statistical analyses to the SA code
</commit_message>
<xml_diff>
--- a/data/saDataset.xlsx
+++ b/data/saDataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="16">
   <si>
     <t>timePoint</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>pc</t>
+  </si>
+  <si>
+    <t>ps</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
         <v>1.103396667</v>
       </c>
       <c r="J2" s="4">
-        <f t="shared" ref="J2:J83" si="2">3/I2</f>
+        <f t="shared" ref="J2:J90" si="2">3/I2</f>
         <v>2.718877164</v>
       </c>
       <c r="K2" s="3">
@@ -2149,116 +2152,425 @@
       </c>
     </row>
     <row r="50">
-      <c r="I50" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J50" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A50" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D50" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.761492</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0.766028</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0.756092</v>
+      </c>
+      <c r="I50" s="4">
+        <f t="shared" si="1"/>
+        <v>0.761204</v>
+      </c>
+      <c r="J50" s="4">
+        <f t="shared" si="2"/>
+        <v>3.94112485</v>
+      </c>
+      <c r="K50" s="3">
+        <v>190.016739</v>
       </c>
     </row>
     <row r="51">
-      <c r="I51" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J51" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A51" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="D51" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.916156</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0.916612</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0.901219</v>
+      </c>
+      <c r="I51" s="4">
+        <f t="shared" si="1"/>
+        <v>0.911329</v>
+      </c>
+      <c r="J51" s="4">
+        <f t="shared" si="2"/>
+        <v>3.291895682</v>
+      </c>
+      <c r="K51" s="3">
+        <v>103.633705</v>
       </c>
     </row>
     <row r="52">
-      <c r="I52" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J52" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A52" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="D52" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1.54855</v>
+      </c>
+      <c r="G52" s="3">
+        <v>1.54116</v>
+      </c>
+      <c r="H52" s="3">
+        <v>1.53285</v>
+      </c>
+      <c r="I52" s="4">
+        <f t="shared" si="1"/>
+        <v>1.540853333</v>
+      </c>
+      <c r="J52" s="4">
+        <f t="shared" si="2"/>
+        <v>1.946973106</v>
+      </c>
+      <c r="K52" s="3">
+        <v>177.580276</v>
       </c>
     </row>
     <row r="53">
-      <c r="I53" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J53" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A53" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1.56975</v>
+      </c>
+      <c r="G53" s="3">
+        <v>1.56975</v>
+      </c>
+      <c r="H53" s="3">
+        <v>1.56975</v>
+      </c>
+      <c r="I53" s="4">
+        <f t="shared" si="1"/>
+        <v>1.56975</v>
+      </c>
+      <c r="J53" s="4">
+        <f t="shared" si="2"/>
+        <v>1.911132346</v>
+      </c>
+      <c r="K53" s="3">
+        <v>252.151855</v>
       </c>
     </row>
     <row r="54">
-      <c r="I54" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J54" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A54" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="D54" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="3">
+        <v>6.5366</v>
+      </c>
+      <c r="G54" s="3">
+        <v>6.51526</v>
+      </c>
+      <c r="H54" s="3">
+        <v>6.49434</v>
+      </c>
+      <c r="I54" s="4">
+        <f t="shared" si="1"/>
+        <v>6.5154</v>
+      </c>
+      <c r="J54" s="4">
+        <f t="shared" si="2"/>
+        <v>0.460447555</v>
+      </c>
+      <c r="K54" s="3">
+        <v>280.506165</v>
       </c>
     </row>
     <row r="55">
-      <c r="I55" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J55" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A55" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D55" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.478508</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0.482802</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0.48883</v>
+      </c>
+      <c r="I55" s="4">
+        <f t="shared" si="1"/>
+        <v>0.48338</v>
+      </c>
+      <c r="J55" s="4">
+        <f t="shared" si="2"/>
+        <v>6.206297323</v>
+      </c>
+      <c r="K55" s="3">
+        <v>135.365265</v>
       </c>
     </row>
     <row r="56">
-      <c r="I56" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J56" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A56" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="D56" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1.82289</v>
+      </c>
+      <c r="G56" s="3">
+        <v>1.84345</v>
+      </c>
+      <c r="H56" s="3">
+        <v>1.87992</v>
+      </c>
+      <c r="I56" s="4">
+        <f t="shared" si="1"/>
+        <v>1.848753333</v>
+      </c>
+      <c r="J56" s="4">
+        <f t="shared" si="2"/>
+        <v>1.622715127</v>
+      </c>
+      <c r="K56" s="3">
+        <v>34.749279</v>
       </c>
     </row>
     <row r="57">
-      <c r="I57" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J57" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A57" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="D57" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1.25343</v>
+      </c>
+      <c r="G57" s="3">
+        <v>1.26447</v>
+      </c>
+      <c r="H57" s="3">
+        <v>1.25494</v>
+      </c>
+      <c r="I57" s="4">
+        <f t="shared" si="1"/>
+        <v>1.257613333</v>
+      </c>
+      <c r="J57" s="4">
+        <f t="shared" si="2"/>
+        <v>2.385470892</v>
+      </c>
+      <c r="K57" s="3">
+        <v>87.473793</v>
       </c>
     </row>
     <row r="58">
-      <c r="I58" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J58" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A58" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D58" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="3">
+        <v>1.33362</v>
+      </c>
+      <c r="G58" s="3">
+        <v>1.33067</v>
+      </c>
+      <c r="H58" s="3">
+        <v>1.34269</v>
+      </c>
+      <c r="I58" s="4">
+        <f t="shared" si="1"/>
+        <v>1.33566</v>
+      </c>
+      <c r="J58" s="4">
+        <f t="shared" si="2"/>
+        <v>2.246080589</v>
+      </c>
+      <c r="K58" s="3">
+        <v>140.08075</v>
       </c>
     </row>
     <row r="59">
-      <c r="I59" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J59" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A59" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="D59" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="3">
+        <v>1.07647</v>
+      </c>
+      <c r="G59" s="3">
+        <v>1.07574</v>
+      </c>
+      <c r="H59" s="3">
+        <v>1.08931</v>
+      </c>
+      <c r="I59" s="4">
+        <f t="shared" si="1"/>
+        <v>1.080506667</v>
+      </c>
+      <c r="J59" s="4">
+        <f t="shared" si="2"/>
+        <v>2.776475234</v>
+      </c>
+      <c r="K59" s="3">
+        <v>191.489624</v>
       </c>
     </row>
     <row r="60">
-      <c r="I60" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J60" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="A60" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D60" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="3">
+        <v>2.93244</v>
+      </c>
+      <c r="G60" s="3">
+        <v>2.89922</v>
+      </c>
+      <c r="H60" s="3">
+        <v>2.92458</v>
+      </c>
+      <c r="I60" s="4">
+        <f t="shared" si="1"/>
+        <v>2.918746667</v>
+      </c>
+      <c r="J60" s="4">
+        <f t="shared" si="2"/>
+        <v>1.027838433</v>
       </c>
     </row>
     <row r="61">
+      <c r="A61" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="D61" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I61" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2269,6 +2581,21 @@
       </c>
     </row>
     <row r="62">
+      <c r="A62" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="D62" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I62" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2279,6 +2606,21 @@
       </c>
     </row>
     <row r="63">
+      <c r="A63" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D63" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I63" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2289,6 +2631,21 @@
       </c>
     </row>
     <row r="64">
+      <c r="A64" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="D64" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I64" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2299,6 +2656,21 @@
       </c>
     </row>
     <row r="65">
+      <c r="A65" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D65" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I65" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2309,6 +2681,21 @@
       </c>
     </row>
     <row r="66">
+      <c r="A66" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="D66" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I66" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2319,6 +2706,21 @@
       </c>
     </row>
     <row r="67">
+      <c r="A67" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="D67" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I67" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2329,6 +2731,21 @@
       </c>
     </row>
     <row r="68">
+      <c r="A68" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D68" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I68" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2339,6 +2756,21 @@
       </c>
     </row>
     <row r="69">
+      <c r="A69" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="D69" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I69" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2349,6 +2781,21 @@
       </c>
     </row>
     <row r="70">
+      <c r="A70" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D70" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="I70" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2359,6 +2806,21 @@
       </c>
     </row>
     <row r="71">
+      <c r="A71" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="D71" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="I71" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2369,6 +2831,21 @@
       </c>
     </row>
     <row r="72">
+      <c r="A72" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="D72" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="I72" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2379,6 +2856,21 @@
       </c>
     </row>
     <row r="73">
+      <c r="A73" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D73" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="I73" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2389,6 +2881,21 @@
       </c>
     </row>
     <row r="74">
+      <c r="A74" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="D74" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="I74" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2399,6 +2906,21 @@
       </c>
     </row>
     <row r="75">
+      <c r="A75" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D75" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I75" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2409,6 +2931,21 @@
       </c>
     </row>
     <row r="76">
+      <c r="A76" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="D76" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I76" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2419,6 +2956,21 @@
       </c>
     </row>
     <row r="77">
+      <c r="A77" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="D77" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I77" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2429,6 +2981,21 @@
       </c>
     </row>
     <row r="78">
+      <c r="A78" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D78" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I78" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2439,6 +3006,21 @@
       </c>
     </row>
     <row r="79">
+      <c r="A79" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="D79" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I79" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2449,6 +3031,21 @@
       </c>
     </row>
     <row r="80">
+      <c r="A80" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D80" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I80" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2459,6 +3056,21 @@
       </c>
     </row>
     <row r="81">
+      <c r="A81" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="D81" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I81" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2469,6 +3081,21 @@
       </c>
     </row>
     <row r="82">
+      <c r="A82" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="D82" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I82" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2479,6 +3106,21 @@
       </c>
     </row>
     <row r="83">
+      <c r="A83" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D83" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I83" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -2489,44 +3131,163 @@
       </c>
     </row>
     <row r="84">
+      <c r="A84" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="D84" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I84" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="J84" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="85">
+      <c r="A85" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="D85" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I85" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="J85" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="86">
+      <c r="A86" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="D86" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I86" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="J86" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="87">
+      <c r="A87" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="D87" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I87" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="J87" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="88">
+      <c r="A88" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="D88" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I88" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="J88" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="89">
+      <c r="A89" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="D89" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I89" s="4" t="str">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="J89" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="90">
+      <c r="A90" s="3"/>
       <c r="I90" s="4" t="str">
         <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J90" s="4" t="str">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated code, added species to lmer tests
</commit_message>
<xml_diff>
--- a/data/saDataset.xlsx
+++ b/data/saDataset.xlsx
@@ -8,6 +8,8 @@
     <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Sheet4" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Sheet5" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Sheet6" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Sheet7" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="46">
   <si>
     <t>timePoint</t>
   </si>
@@ -145,6 +147,15 @@
   <si>
     <t>PS07</t>
   </si>
+  <si>
+    <t>percentChange</t>
+  </si>
+  <si>
+    <t>speciesPercentChange</t>
+  </si>
+  <si>
+    <t>meanPercentChange</t>
+  </si>
 </sst>
 </file>
 
@@ -210,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
     <border>
       <left style="thin">
@@ -226,11 +237,14 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <right/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -274,6 +288,9 @@
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -299,6 +316,14 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2117,14 +2142,14 @@
         <f t="shared" si="2"/>
         <v>1.914485669</v>
       </c>
-      <c r="L35" s="6">
-        <v>78.328491</v>
+      <c r="L35" s="4">
+        <v>75.916962</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="7">
         <f>L120-L35</f>
-        <v>101.301575</v>
+        <v>103.713104</v>
       </c>
     </row>
     <row r="36">
@@ -11309,4 +11334,897 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="11">
+        <v>51.1666436</v>
+      </c>
+      <c r="E2" s="12">
+        <f t="shared" ref="E2:E3" si="1">AVERAGE(D2,D4,D6)</f>
+        <v>51.70638957</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="11">
+        <v>2.0785674</v>
+      </c>
+      <c r="E3" s="12">
+        <f t="shared" si="1"/>
+        <v>6.4214963</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="11">
+        <v>59.0793079</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.4578967</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="11">
+        <v>44.8732172</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="11">
+        <v>16.7280248</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="11">
+        <v>96.0458673</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" ref="E8:E9" si="2">AVERAGE(D8,D10,D12)</f>
+        <v>84.2619502</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1.8459165</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" si="2"/>
+        <v>2.949500667</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="11">
+        <v>88.1911478</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="11">
+        <v>1.2408509</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="11">
+        <v>68.5488355</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="11">
+        <v>5.7617346</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="11">
+        <v>54.3126703</v>
+      </c>
+      <c r="E14" s="12">
+        <f t="shared" ref="E14:E15" si="3">AVERAGE(D14,D16,D18,D20,D22)</f>
+        <v>50.74009748</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="11">
+        <v>12.1239379</v>
+      </c>
+      <c r="E15" s="12">
+        <f t="shared" si="3"/>
+        <v>12.08804534</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="11">
+        <v>55.6645262</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="11">
+        <v>7.4648945</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="11">
+        <v>15.1580479</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0.9131002</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="11">
+        <v>64.059561</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="11">
+        <v>17.7393166</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="11">
+        <v>64.505682</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="11">
+        <v>22.1989775</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="11">
+        <v>146.1005032</v>
+      </c>
+      <c r="E24" s="12">
+        <f t="shared" ref="E24:E25" si="4">AVERAGE(D24,D26,D28)</f>
+        <v>141.203227</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="11">
+        <v>5.856935</v>
+      </c>
+      <c r="E25" s="12">
+        <f t="shared" si="4"/>
+        <v>21.11020413</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="11">
+        <v>169.8694792</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="11">
+        <v>15.1209077</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="11">
+        <v>107.6396987</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="11">
+        <v>42.3527697</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="11">
+        <v>163.8379922</v>
+      </c>
+      <c r="E30" s="12">
+        <f t="shared" ref="E30:E31" si="5">AVERAGE(D30,D32,D34)</f>
+        <v>130.9937838</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="11">
+        <v>3.0760581</v>
+      </c>
+      <c r="E31" s="12">
+        <f t="shared" si="5"/>
+        <v>6.297888233</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="11">
+        <v>124.3915344</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="11">
+        <v>7.7228451</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="11">
+        <v>104.7518247</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="11">
+        <v>8.0947615</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="11">
+        <v>125.371513</v>
+      </c>
+      <c r="E36" s="12">
+        <f t="shared" ref="E36:E37" si="6">AVERAGE(D36,D38,D40,D42,D44)</f>
+        <v>115.1767128</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="11">
+        <v>21.2991977</v>
+      </c>
+      <c r="E37" s="12">
+        <f t="shared" si="6"/>
+        <v>20.91861092</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="11">
+        <v>122.0985346</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="11">
+        <v>24.5933846</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="11">
+        <v>82.1257943</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="11">
+        <v>1.4566994</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="11">
+        <v>122.9692483</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="11">
+        <v>18.6198474</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="11">
+        <v>123.3184736</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="11">
+        <v>38.6239255</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3">
+        <v>51.706389566666665</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6.4214963</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="12">
+        <v>84.2619502</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="12">
+        <v>2.9495006666666668</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="12">
+        <v>50.740097479999996</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12">
+        <v>12.088045339999999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="12">
+        <v>141.20322703333332</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="12">
+        <v>21.110204133333337</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="12">
+        <v>130.99378376666667</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="12">
+        <v>6.297888233333334</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="12">
+        <v>115.17671276000002</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="12">
+        <v>20.91861092</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>